<commit_message>
Handle reserved field in union.
</commit_message>
<xml_diff>
--- a/register_printer/tests/dataset/dataset1/excels/block1.xlsx
+++ b/register_printer/tests/dataset/dataset1/excels/block1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\git\RegisterPrinter\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangpe/git/RegisterPrinter/register_printer/tests/dataset/dataset1/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2E554B-025D-46F2-A008-6196D2BDA2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBA2891-EFF6-F84D-9B13-406A7A8D02AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="900" windowWidth="22110" windowHeight="14170" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
+    <workbookView xWindow="6680" yWindow="900" windowWidth="22120" windowHeight="14180" activeTab="1" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>0x0</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -327,6 +327,9 @@
   <si>
     <t>Field9</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -337,14 +340,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -353,14 +356,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -369,7 +372,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -424,7 +427,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,7 +460,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -755,22 +758,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4915A7C1-6506-4C54-966C-F795DE988BD6}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="18.25" customWidth="1"/>
-    <col min="5" max="5" width="14.25" customWidth="1"/>
-    <col min="6" max="6" width="12.08203125" customWidth="1"/>
+    <col min="3" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -778,15 +781,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -806,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -826,7 +829,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -846,12 +849,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -877,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -888,7 +891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>7</v>
       </c>
@@ -908,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>10</v>
       </c>
@@ -928,7 +931,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -939,7 +942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>7</v>
       </c>
@@ -959,7 +962,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>12</v>
       </c>
@@ -979,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -990,7 +993,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>3</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>14</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>10</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>31</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>11</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28">
         <v>15</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31">
         <v>10</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C32">
         <v>31</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35">
         <v>10</v>
       </c>
@@ -1230,18 +1233,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D33A049-DC09-4FC1-9AD2-1B7B43D86792}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1252,12 +1255,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1302,10 +1305,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1314,7 +1317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>10</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>7</v>
       </c>
@@ -1365,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Update dataset1 and json baseline.
</commit_message>
<xml_diff>
--- a/register_printer/tests/dataset/dataset1/excels/block1.xlsx
+++ b/register_printer/tests/dataset/dataset1/excels/block1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\git\RegisterPrinter\register_printer\tests\dataset\dataset1\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45558AEB-7EB5-4A17-BC99-2538D182B0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE4200C-EA53-4DDB-B985-76CAE5986F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="3800" windowWidth="28800" windowHeight="15360" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
+    <workbookView xWindow="2030" yWindow="4770" windowWidth="19940" windowHeight="15360" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="1" r:id="rId1"/>
@@ -214,10 +214,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Field8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Field9</t>
   </si>
   <si>
@@ -327,6 +323,10 @@
   </si>
   <si>
     <t>REG_A2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -757,7 +757,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -773,7 +773,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -815,16 +815,16 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -841,15 +841,15 @@
         <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -872,7 +872,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
         <v>23</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -982,10 +982,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
         <v>41</v>
@@ -1036,10 +1036,10 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1056,10 +1056,10 @@
         <v>39</v>
       </c>
       <c r="G23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1076,21 +1076,21 @@
         <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1101,16 +1101,16 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1121,27 +1121,27 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
       <c r="H30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1158,10 +1158,10 @@
         <v>39</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1178,18 +1178,18 @@
         <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1200,23 +1200,23 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
       </c>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F21 F23:F25 F27:F29 F31:F33 F35" xr:uid="{4096D060-3F28-4448-80C0-EA07DD153096}">
-      <formula1>"RW, RO,RS,RC,W1C,WO,WRS,WRC"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F35" xr:uid="{EA86D225-F788-48D8-BBE3-273BFCAFA5D9}">
+      <formula1>"RW, RO,RS,RC,W1C,WO,WRS,WRC,-"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1244,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I1" t="s">
         <v>14</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1278,7 +1278,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>23</v>
@@ -1303,10 +1303,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>

</xml_diff>